<commit_message>
Remove unused column and between blank columns from "good" spread sheet.
Also, remove corresponding heading check from code.
</commit_message>
<xml_diff>
--- a/tests/data/spread-sheet/good.xlsx
+++ b/tests/data/spread-sheet/good.xlsx
@@ -20,15 +20,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
   <si>
     <t xml:space="preserve">ControlId</t>
   </si>
   <si>
     <t xml:space="preserve">ControlText</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ResourceCategory</t>
   </si>
   <si>
     <t xml:space="preserve">Version</t>
@@ -54,28 +51,28 @@
     <t xml:space="preserve">Check whether the EU supported setting is enabled in account settings</t>
   </si>
   <si>
+    <t xml:space="preserve">CM-2</t>
+  </si>
+  <si>
     <t xml:space="preserve">SYSTEM</t>
   </si>
   <si>
-    <t xml:space="preserve">CM-2</t>
-  </si>
-  <si>
     <t xml:space="preserve">Check whether Cloudant has no more than # users with the IAM administrator role</t>
   </si>
   <si>
+    <t xml:space="preserve">AC-2: (j)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC-5: (b)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AC-6</t>
+  </si>
+  <si>
     <t xml:space="preserve">CLOUDANT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC-2: (j)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC-3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC-5: (b)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC-6</t>
   </si>
   <si>
     <t xml:space="preserve">cloudant_admin_role_user_maxcount</t>
@@ -168,22 +165,22 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">AC-17 (2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC-8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC-8 (1)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC-13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC-23</t>
+  </si>
+  <si>
     <t xml:space="preserve">CIS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">AC-17 (2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC-8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC-8 (1)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC-13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SC-23</t>
   </si>
   <si>
     <t xml:space="preserve">cis_tls_configured</t>
@@ -230,9 +227,6 @@
     <t xml:space="preserve">Check whether Virtual Private Cloud (VPC) security groups have no inbound ports open to the internet (0.0.0.0/0)</t>
   </si>
   <si>
-    <t xml:space="preserve">NETWORKING</t>
-  </si>
-  <si>
     <t xml:space="preserve">AC-4</t>
   </si>
   <si>
@@ -275,16 +269,16 @@
     <t xml:space="preserve">Check whether Continuous Delivery toolchain continuously scans source code to identify vulnerabilities above the # threshold. </t>
   </si>
   <si>
+    <t xml:space="preserve">RA-5(a) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI-2(2)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SI-7(1)</t>
+  </si>
+  <si>
     <t xml:space="preserve">TOOLCHAIN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">RA-5(a) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI-2(2)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SI-7(1)</t>
   </si>
   <si>
     <t xml:space="preserve">continuous_delivery_toolchain_sourcecode_scan_severity_configured</t>
@@ -300,10 +294,10 @@
     <t xml:space="preserve">Check whether App ID email verification is enabled for Cloud Directory users</t>
   </si>
   <si>
+    <t xml:space="preserve">none</t>
+  </si>
+  <si>
     <t xml:space="preserve">APPID</t>
-  </si>
-  <si>
-    <t xml:space="preserve">none</t>
   </si>
   <si>
     <t xml:space="preserve">appid_</t>
@@ -586,24 +580,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AS11"/>
+  <dimension ref="A1:N11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AO1" activeCellId="0" sqref="AO1"/>
+      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="14.31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="18.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="18.89"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="19.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="39.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="20.98"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="24.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="39.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="20.98"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="49.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,32 +602,29 @@
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="D1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AD1" s="4"/>
-      <c r="AE1" s="4"/>
-      <c r="AF1" s="4"/>
-      <c r="AG1" s="4"/>
-      <c r="AH1" s="4"/>
-      <c r="AI1" s="4"/>
-      <c r="AM1" s="4" t="s">
+      <c r="L1" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="AN1" s="5" t="s">
+      <c r="M1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="AR1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>7</v>
-      </c>
-      <c r="AS1" s="6" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -646,65 +632,59 @@
         <v>3000036</v>
       </c>
       <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="9" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="10"/>
+      <c r="G2" s="10"/>
+      <c r="H2" s="10"/>
+      <c r="K2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="AB2" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC2" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD2" s="10"/>
-      <c r="AE2" s="10"/>
-      <c r="AF2" s="10"/>
-      <c r="AG2" s="10"/>
-      <c r="AM2" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="AN2" s="10"/>
-      <c r="AR2" s="10"/>
-      <c r="AS2" s="10"/>
+      <c r="L2" s="10"/>
+      <c r="M2" s="10"/>
+      <c r="N2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>3000109</v>
       </c>
       <c r="B3" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="I3" s="9" t="s">
+      <c r="E3" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AB3" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="12" t="s">
+      <c r="F3" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="AE3" s="10" t="s">
+      <c r="H3" s="13"/>
+      <c r="K3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="AF3" s="10" t="s">
+      <c r="L3" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="AG3" s="13"/>
-      <c r="AM3" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN3" s="10" t="s">
+      <c r="M3" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="AR3" s="14" t="s">
+      <c r="N3" s="10" t="s">
         <v>19</v>
-      </c>
-      <c r="AS3" s="10" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -712,38 +692,35 @@
         <v>3000110</v>
       </c>
       <c r="B4" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="H4" s="13"/>
+      <c r="K4" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB4" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC4" s="12" t="s">
-        <v>14</v>
-      </c>
-      <c r="AD4" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="AE4" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="AF4" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="AG4" s="13"/>
-      <c r="AM4" s="11" t="s">
-        <v>13</v>
-      </c>
-      <c r="AN4" s="10" t="s">
+      <c r="M4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="AR4" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="AS4" s="10" t="s">
-        <v>20</v>
+      <c r="N4" s="10" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="111.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -751,79 +728,73 @@
         <v>3000403</v>
       </c>
       <c r="B5" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="I5" s="9" t="s">
+      <c r="E5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC5" s="13" t="s">
+      <c r="F5" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AD5" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="AE5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="AF5" s="10" t="s">
+      <c r="K5" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AG5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="AM5" s="11" t="s">
-        <v>25</v>
-      </c>
-      <c r="AN5" s="10" t="s">
+      <c r="M5" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="AR5" s="16" t="s">
-        <v>32</v>
-      </c>
-      <c r="AS5" s="10"/>
+      <c r="N5" s="10"/>
     </row>
     <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
         <v>3000409</v>
       </c>
       <c r="B6" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>26</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K6" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB6" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC6" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="AE6" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="AF6" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="AG6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM6" s="11" t="s">
+      <c r="L6" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="AN6" s="10" t="s">
+      <c r="M6" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="AR6" s="14" t="s">
+      <c r="N6" s="10" t="s">
         <v>36</v>
-      </c>
-      <c r="AS6" s="10" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -831,112 +802,103 @@
         <v>3000410</v>
       </c>
       <c r="B7" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="C7" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="I7" s="9" t="s">
+      <c r="E7" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="F7" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="AB7" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC7" s="13" t="s">
+      <c r="G7" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="AD7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="AE7" s="10" t="s">
+      <c r="H7" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="AF7" s="10" t="s">
+      <c r="K7" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AG7" s="10" t="s">
+      <c r="L7" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="AM7" s="11" t="s">
-        <v>44</v>
-      </c>
-      <c r="AN7" s="10" t="s">
-        <v>45</v>
-      </c>
-      <c r="AR7" s="10"/>
-      <c r="AS7" s="10"/>
+      <c r="M7" s="10"/>
+      <c r="N7" s="10"/>
     </row>
     <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
         <v>3000450</v>
       </c>
       <c r="B8" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D8" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E8" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F8" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="I8" s="9" t="s">
-        <v>10</v>
-      </c>
-      <c r="AB8" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC8" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="AD8" s="10" t="s">
+      <c r="G8" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="AE8" s="10" t="s">
+      <c r="H8" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="AF8" s="10" t="s">
+      <c r="K8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="AG8" s="10" t="s">
+      <c r="L8" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="AM8" s="11" t="s">
-        <v>51</v>
-      </c>
-      <c r="AN8" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR8" s="10"/>
-      <c r="AS8" s="10"/>
+      <c r="M8" s="10"/>
+      <c r="N8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
         <v>3000603</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C9" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="E9" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="I9" s="9" t="s">
+      <c r="G9" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="AB9" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC9" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AD9" s="10" t="s">
+      <c r="H9" s="10"/>
+      <c r="K9" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="AE9" s="10" t="s">
+      <c r="L9" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="AF9" s="10" t="s">
+      <c r="M9" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="AG9" s="10"/>
-      <c r="AM9" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN9" s="10" t="s">
+      <c r="N9" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="AR9" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS9" s="19" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -944,66 +906,60 @@
         <v>3000721</v>
       </c>
       <c r="B10" s="8" t="s">
+        <v>59</v>
+      </c>
+      <c r="C10" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E10" s="10"/>
+      <c r="F10" s="10"/>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="K10" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="I10" s="9" t="s">
+      <c r="L10" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="AB10" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC10" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="AD10" s="10"/>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="10"/>
-      <c r="AG10" s="10"/>
-      <c r="AM10" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="AN10" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="AR10" s="10"/>
-      <c r="AS10" s="10"/>
+      <c r="M10" s="10"/>
+      <c r="N10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
         <v>9000101</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>65</v>
-      </c>
-      <c r="I11" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="AB11" s="9" t="n">
-        <v>1</v>
-      </c>
-      <c r="AC11" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="AD11" s="9"/>
-      <c r="AE11" s="9"/>
-      <c r="AF11" s="9"/>
-      <c r="AG11" s="10"/>
-      <c r="AM11" s="18" t="s">
-        <v>54</v>
-      </c>
-      <c r="AN11" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="C11" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
+      <c r="K11" s="18" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="M11" s="16" t="s">
+        <v>57</v>
+      </c>
+      <c r="N11" s="19" t="s">
         <v>58</v>
-      </c>
-      <c r="AR11" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="AS11" s="19" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="AC1:AI1"/>
+    <mergeCell ref="D1:J1"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
feat: xlsx filter (#1050)
* Check for xlsx-to-profile required config vars.

* Support for filter-column.

* Feat/xlsx filter.

* Fix code review items.
</commit_message>
<xml_diff>
--- a/tests/data/spread-sheet/good.xlsx
+++ b/tests/data/spread-sheet/good.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
   <si>
     <t xml:space="preserve">ControlId</t>
   </si>
@@ -46,6 +46,9 @@
   <si>
     <t xml:space="preserve">Values
 default , [alternatives]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Include in FS Cloud Profile?</t>
   </si>
   <si>
     <t xml:space="preserve">Check whether the EU supported setting is enabled in account settings</t>
@@ -104,6 +107,9 @@
     <t xml:space="preserve">3, []</t>
   </si>
   <si>
+    <t xml:space="preserve">YES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check whether Cloudant has no more than # service IDs with the IAM administrator role</t>
   </si>
   <si>
@@ -131,6 +137,9 @@
       </rPr>
       <t xml:space="preserve">no_of_service_id_admins_for_cloudant_db</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">no</t>
   </si>
   <si>
     <r>
@@ -190,6 +199,9 @@
 cis_tls_versions</t>
   </si>
   <si>
+    <t xml:space="preserve">NO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Check whether Kubernetes Service Ingress is configured only with TLS v1.2 for all inbound traffic</t>
   </si>
   <si>
@@ -243,6 +255,9 @@
   </si>
   <si>
     <t xml:space="preserve">vpc_no_inbound_ports_public</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">Check whether Kubernetes Service version is up-to-date</t>
@@ -576,17 +591,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M1" activeCellId="0" sqref="M1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="P8" activeCellId="0" sqref="P8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.06"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.78"/>
@@ -626,65 +641,74 @@
       <c r="N1" s="6" t="s">
         <v>7</v>
       </c>
+      <c r="O1" s="6"/>
+      <c r="P1" s="5" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="n">
         <v>3000036</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C2" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E2" s="10"/>
       <c r="F2" s="10"/>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="K2" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="L2" s="10"/>
       <c r="M2" s="10"/>
       <c r="N2" s="10"/>
+      <c r="O2" s="10"/>
     </row>
     <row r="3" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="7" t="n">
         <v>3000109</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C3" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D3" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G3" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="13"/>
       <c r="K3" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" s="10" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M3" s="14" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="N3" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O3" s="10"/>
+      <c r="P3" s="0" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -692,35 +716,39 @@
         <v>3000110</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C4" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="10" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G4" s="10" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="13"/>
       <c r="K4" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L4" s="10" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="M4" s="14" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="N4" s="10" t="s">
-        <v>19</v>
+        <v>20</v>
+      </c>
+      <c r="O4" s="10"/>
+      <c r="P4" s="0" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="111.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -728,234 +756,247 @@
         <v>3000403</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C5" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D5" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H5" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="L5" s="10" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="M5" s="16" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N5" s="10"/>
+      <c r="O5" s="10"/>
+      <c r="P5" s="0" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
         <v>3000409</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C6" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="13" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E6" s="10" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F6" s="10" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="G6" s="10" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="H6" s="10" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K6" s="11" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="L6" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="M6" s="14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="N6" s="10" t="s">
-        <v>36</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="O6" s="10"/>
     </row>
     <row r="7" customFormat="false" ht="102.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
         <v>3000410</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="E7" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="F7" s="10" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="G7" s="10" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="H7" s="10" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="K7" s="11" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="L7" s="10" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="M7" s="10"/>
       <c r="N7" s="10"/>
+      <c r="O7" s="10"/>
+      <c r="P7" s="0" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="7" t="n">
         <v>3000450</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="C8" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E8" s="10" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="F8" s="10" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="H8" s="10" t="s">
-        <v>48</v>
+        <v>53</v>
       </c>
       <c r="K8" s="11" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="M8" s="10"/>
       <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
     </row>
     <row r="9" customFormat="false" ht="144.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="7" t="n">
         <v>3000603</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="C9" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D9" s="13" t="s">
-        <v>47</v>
+        <v>52</v>
       </c>
       <c r="E9" s="10" t="s">
-        <v>52</v>
+        <v>57</v>
       </c>
       <c r="F9" s="10" t="s">
-        <v>53</v>
+        <v>58</v>
       </c>
       <c r="G9" s="10" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H9" s="10"/>
       <c r="K9" s="18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L9" s="10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M9" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="N9" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" customFormat="false" ht="79.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="7" t="n">
         <v>3000721</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>59</v>
+        <v>64</v>
       </c>
       <c r="C10" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="E10" s="10"/>
       <c r="F10" s="10"/>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="K10" s="11" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="L10" s="10" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="M10" s="10"/>
       <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
     </row>
     <row r="11" customFormat="false" ht="73.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="7" t="n">
         <v>9000101</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="C11" s="9" t="n">
         <v>1</v>
       </c>
       <c r="D11" s="13" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
       <c r="G11" s="9"/>
       <c r="H11" s="10"/>
       <c r="K11" s="18" t="s">
-        <v>55</v>
+        <v>60</v>
       </c>
       <c r="L11" s="10" t="s">
-        <v>56</v>
+        <v>61</v>
       </c>
       <c r="M11" s="16" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="N11" s="19" t="s">
-        <v>58</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="O11" s="19"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>